<commit_message>
Changes from feedback on week 46.
</commit_message>
<xml_diff>
--- a/src/fysisk_biokemi/datasets/files/dialys-exper.xlsx
+++ b/src/fysisk_biokemi/datasets/files/dialys-exper.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/au616397/Library/CloudStorage/Dropbox/mbg/fysisk_biokemi/fysisk_biokemi/src/fysisk_biokemi/datasets/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C5E3AB-AFFF-C74B-838E-FC3AC39A116A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BFF29E-F16E-9A46-9EA4-849E903CD414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27520" windowHeight="16940" xr2:uid="{4F9DEF64-D795-B34B-9869-34DF6B65F3AE}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Free ligand [L](µM)</t>
+    <t>Free_ligand_(uM)</t>
   </si>
   <si>
-    <t>n-bar</t>
+    <t>n_bar</t>
   </si>
 </sst>
 </file>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6F5CB2B-899A-6F4A-8ADF-EF5A3B0BF94D}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>